<commit_message>
finalized cb table. new fornew format for tbl footnotes
</commit_message>
<xml_diff>
--- a/archive/table_drafts.xlsx
+++ b/archive/table_drafts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kudrzycb/polybox/Youth Employment/2 CQP/Paper/archive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F827A2-B6A7-3D46-9462-5E9A9E5EA7E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8AD4AC-8FFC-ED4F-90CA-56F7DFE023D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="440" windowWidth="28800" windowHeight="16000" activeTab="1" xr2:uid="{1D26E68A-A2BA-0245-8976-741BB00BC1B0}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="75">
   <si>
     <t>Category</t>
   </si>
@@ -236,6 +236,21 @@
   </si>
   <si>
     <t>max 1 out of 2 from baseline</t>
+  </si>
+  <si>
+    <t>| Status        | Explanation                                                                                                                                            | Youth Survey Sampling                                                                                         | Firm Survey Sampling                                                                                          |</t>
+  </si>
+  <si>
+    <t>|---------------|--------------------------------------------------------------------------------------------------------------------------------------------------------|---------------------------------------------------------------------------------------------------------------|---------------------------------------------------------------------------------------------------------------|</t>
+  </si>
+  <si>
+    <t>| Selected      | Already in apprenticeship, applied via master craftsmen. Passed exam and selected.                                                                     | Random sampling from list of all CQP  applicants in five chosen trades and geographic region (Southern Benin) | If more than one CQP applicant training in firm, at most two apprentices were  randomly selected at baseline. |</t>
+  </si>
+  <si>
+    <t>| Not selected  | Already in apprenticeship, applied via master craftsmen. Not selected (training center proximity or exam score). Continued traditional apprenticeship. | Random sampling from list of all CQP  applicants in five chosen trades and geographic region (Southern Benin) | If more than one CQP applicant training in firm, at most two apprentices were  randomly selected at baseline. |</t>
+  </si>
+  <si>
+    <t>| Did not apply | Did not apply to CQP. Trained as traditional apprentice.                                                                                               |  N/A                                                                                                          | Firm owner lists 5 apprentices who did not apply to CQP. One randomly selected at baseline.                   |</t>
   </si>
 </sst>
 </file>
@@ -286,6 +301,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -293,9 +311,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -689,19 +704,19 @@
       </c>
     </row>
     <row r="6" spans="2:17">
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="2:17">
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="5"/>
+      <c r="M7" s="6"/>
       <c r="O7" t="s">
         <v>16</v>
       </c>
@@ -745,10 +760,10 @@
       <c r="E9" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="4">
         <v>20</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="4">
         <v>12</v>
       </c>
       <c r="N9" t="s">
@@ -765,8 +780,8 @@
       <c r="E10" t="s">
         <v>14</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
       <c r="N10" t="s">
         <v>20</v>
       </c>
@@ -781,15 +796,15 @@
       <c r="E11" t="s">
         <v>15</v>
       </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
       <c r="N11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:17">
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
       <c r="O12" t="s">
         <v>16</v>
       </c>
@@ -812,10 +827,10 @@
       </c>
     </row>
     <row r="14" spans="2:17">
-      <c r="L14" s="3">
+      <c r="L14" s="4">
         <v>20</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="M14" s="4" t="s">
         <v>27</v>
       </c>
       <c r="N14" t="s">
@@ -823,15 +838,15 @@
       </c>
     </row>
     <row r="15" spans="2:17">
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
       <c r="N15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:17">
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
       <c r="N16" t="s">
         <v>21</v>
       </c>
@@ -848,10 +863,10 @@
       </c>
     </row>
     <row r="18" spans="6:17">
-      <c r="L18" s="3" t="s">
+      <c r="L18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M18" s="3">
+      <c r="M18" s="4">
         <v>12</v>
       </c>
       <c r="N18" t="s">
@@ -865,8 +880,8 @@
       <c r="G19" t="s">
         <v>32</v>
       </c>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
       <c r="N19" t="s">
         <v>20</v>
       </c>
@@ -875,8 +890,8 @@
       <c r="G20" t="s">
         <v>33</v>
       </c>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
       <c r="N20" t="s">
         <v>21</v>
       </c>
@@ -924,10 +939,10 @@
       <c r="H23" t="s">
         <v>41</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="L23" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M23" s="3" t="s">
+      <c r="M23" s="4" t="s">
         <v>27</v>
       </c>
       <c r="N23" t="s">
@@ -944,15 +959,15 @@
       <c r="H24" t="s">
         <v>40</v>
       </c>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
       <c r="N24" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="6:17">
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
       <c r="N25" t="s">
         <v>21</v>
       </c>
@@ -997,10 +1012,10 @@
       <c r="H28" t="s">
         <v>36</v>
       </c>
-      <c r="L28" s="3" t="s">
+      <c r="L28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M28" s="3" t="s">
+      <c r="M28" s="4" t="s">
         <v>29</v>
       </c>
       <c r="N28" t="s">
@@ -1014,8 +1029,8 @@
       <c r="H29" t="s">
         <v>34</v>
       </c>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
       <c r="N29" t="s">
         <v>20</v>
       </c>
@@ -1027,8 +1042,8 @@
       <c r="H30" t="s">
         <v>36</v>
       </c>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
       <c r="N30" t="s">
         <v>21</v>
       </c>
@@ -1071,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31A7BC2-D259-5943-B5A3-5653F97DB072}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1086,8 +1101,8 @@
     <row r="1" spans="1:9" ht="17" customHeight="1">
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:9">
       <c r="B2" s="2" t="s">
@@ -1202,6 +1217,31 @@
       </c>
       <c r="C14" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sync with nadel laptop
</commit_message>
<xml_diff>
--- a/archive/table_drafts.xlsx
+++ b/archive/table_drafts.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kudrzycb/polybox/Youth Employment/2 CQP/Paper/archive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8AD4AC-8FFC-ED4F-90CA-56F7DFE023D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A6DDBA-6B52-F745-94EB-93D380C23C09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="440" windowWidth="28800" windowHeight="16000" activeTab="1" xr2:uid="{1D26E68A-A2BA-0245-8976-741BB00BC1B0}"/>
+    <workbookView xWindow="4800" yWindow="440" windowWidth="28800" windowHeight="16000" xr2:uid="{1D26E68A-A2BA-0245-8976-741BB00BC1B0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="109">
   <si>
     <t>Category</t>
   </si>
@@ -251,13 +252,115 @@
   </si>
   <si>
     <t>| Did not apply | Did not apply to CQP. Trained as traditional apprentice.                                                                                               |  N/A                                                                                                          | Firm owner lists 5 apprentices who did not apply to CQP. One randomly selected at baseline.                   |</t>
+  </si>
+  <si>
+    <t>By trade, per firm</t>
+  </si>
+  <si>
+    <t>By trade, per app</t>
+  </si>
+  <si>
+    <t>By firm size, per firm</t>
+  </si>
+  <si>
+    <t>By wave/status</t>
+  </si>
+  <si>
+    <t>By status, per app</t>
+  </si>
+  <si>
+    <t>Net benefits</t>
+  </si>
+  <si>
+    <t>Wages by firm size</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>By firm size</t>
+  </si>
+  <si>
+    <t>Firm accounts</t>
+  </si>
+  <si>
+    <t>Projected total, by firm size</t>
+  </si>
+  <si>
+    <t>longtable with assumptions/bounds</t>
+  </si>
+  <si>
+    <t>By status</t>
+  </si>
+  <si>
+    <t>Lost trainer prod.</t>
+  </si>
+  <si>
+    <t>Training expenses</t>
+  </si>
+  <si>
+    <t>By wave/firms size</t>
+  </si>
+  <si>
+    <t>By wave/trade</t>
+  </si>
+  <si>
+    <t>By status, firm side again</t>
+  </si>
+  <si>
+    <t>By status, Firm vs. App side</t>
+  </si>
+  <si>
+    <t>Allowances</t>
+  </si>
+  <si>
+    <t>By wave, trade</t>
+  </si>
+  <si>
+    <t>App prod</t>
+  </si>
+  <si>
+    <t>By trade, firm size</t>
+  </si>
+  <si>
+    <t>By wave, firm vs app side with p-values</t>
+  </si>
+  <si>
+    <t>Fees</t>
+  </si>
+  <si>
+    <t>detailed comp, exp regressions</t>
+  </si>
+  <si>
+    <t>detailed knowledge regressions</t>
+  </si>
+  <si>
+    <t>*change* in scores by trade, firm size</t>
+  </si>
+  <si>
+    <t>*change* in scores by status</t>
+  </si>
+  <si>
+    <t>by status/wave/trade</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>Appendix</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Table</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -269,6 +372,20 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -294,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -302,6 +419,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -314,6 +434,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -628,6 +762,389 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD7C539B-CE9E-BB42-9010-F76F3B23BA63}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21">
+      <c r="A1" s="9"/>
+      <c r="B1" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="21">
+      <c r="A2" s="9"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" ht="21">
+      <c r="A3" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="21">
+      <c r="A4" s="12"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="21">
+      <c r="A5" s="9"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="21">
+      <c r="A6" s="9"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="21">
+      <c r="A7" s="9"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="21">
+      <c r="A8" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="13">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="21">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13">
+        <v>7</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="21">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13">
+        <v>8</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="21">
+      <c r="A11" s="9"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="21">
+      <c r="A12" s="9"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="21">
+      <c r="A13" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="13">
+        <v>7</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="21">
+      <c r="A14" s="9"/>
+      <c r="B14" s="13">
+        <v>8</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="21">
+      <c r="A15" s="9"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="21">
+      <c r="A16" s="9"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="21">
+      <c r="A17" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="13">
+        <v>6</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="21">
+      <c r="A18" s="11"/>
+      <c r="B18" s="13">
+        <v>7</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="21">
+      <c r="A19" s="9"/>
+      <c r="B19" s="13">
+        <v>8</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="21">
+      <c r="A20" s="9"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="21">
+      <c r="A21" s="9"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="21">
+      <c r="A22" s="9"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="21">
+      <c r="A23" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="13">
+        <v>7</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="21">
+      <c r="A24" s="9"/>
+      <c r="B24" s="13">
+        <v>8</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="21">
+      <c r="A25" s="9"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="21">
+      <c r="A26" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="13">
+        <v>7</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="21">
+      <c r="A27" s="9"/>
+      <c r="B27" s="13">
+        <v>8</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="21">
+      <c r="A28" s="9"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="21">
+      <c r="A29" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="13">
+        <v>8</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="21">
+      <c r="A30" s="9"/>
+      <c r="B30" s="13">
+        <v>9</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="21">
+      <c r="A31" s="9"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="21">
+      <c r="A32" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="13">
+        <v>7</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="21">
+      <c r="A33" s="9"/>
+      <c r="B33" s="13">
+        <v>8</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="21">
+      <c r="A34" s="9"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A8:A10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA43DB33-1DEE-0D43-A9B5-67CF5CEB013A}">
   <dimension ref="B1:Q32"/>
   <sheetViews>
@@ -704,19 +1221,19 @@
       </c>
     </row>
     <row r="6" spans="2:17">
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="2:17">
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="6"/>
+      <c r="M7" s="7"/>
       <c r="O7" t="s">
         <v>16</v>
       </c>
@@ -760,10 +1277,10 @@
       <c r="E9" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="5">
         <v>20</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="5">
         <v>12</v>
       </c>
       <c r="N9" t="s">
@@ -780,8 +1297,8 @@
       <c r="E10" t="s">
         <v>14</v>
       </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
       <c r="N10" t="s">
         <v>20</v>
       </c>
@@ -796,15 +1313,15 @@
       <c r="E11" t="s">
         <v>15</v>
       </c>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
       <c r="N11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:17">
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
       <c r="O12" t="s">
         <v>16</v>
       </c>
@@ -827,10 +1344,10 @@
       </c>
     </row>
     <row r="14" spans="2:17">
-      <c r="L14" s="4">
+      <c r="L14" s="5">
         <v>20</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="5" t="s">
         <v>27</v>
       </c>
       <c r="N14" t="s">
@@ -838,15 +1355,15 @@
       </c>
     </row>
     <row r="15" spans="2:17">
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
       <c r="N15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:17">
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
       <c r="N16" t="s">
         <v>21</v>
       </c>
@@ -863,10 +1380,10 @@
       </c>
     </row>
     <row r="18" spans="6:17">
-      <c r="L18" s="4" t="s">
+      <c r="L18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M18" s="5">
         <v>12</v>
       </c>
       <c r="N18" t="s">
@@ -880,8 +1397,8 @@
       <c r="G19" t="s">
         <v>32</v>
       </c>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
       <c r="N19" t="s">
         <v>20</v>
       </c>
@@ -890,8 +1407,8 @@
       <c r="G20" t="s">
         <v>33</v>
       </c>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
       <c r="N20" t="s">
         <v>21</v>
       </c>
@@ -939,10 +1456,10 @@
       <c r="H23" t="s">
         <v>41</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="L23" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="M23" s="5" t="s">
         <v>27</v>
       </c>
       <c r="N23" t="s">
@@ -959,15 +1476,15 @@
       <c r="H24" t="s">
         <v>40</v>
       </c>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
       <c r="N24" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="6:17">
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
       <c r="N25" t="s">
         <v>21</v>
       </c>
@@ -1012,10 +1529,10 @@
       <c r="H28" t="s">
         <v>36</v>
       </c>
-      <c r="L28" s="4" t="s">
+      <c r="L28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M28" s="4" t="s">
+      <c r="M28" s="5" t="s">
         <v>29</v>
       </c>
       <c r="N28" t="s">
@@ -1029,8 +1546,8 @@
       <c r="H29" t="s">
         <v>34</v>
       </c>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
       <c r="N29" t="s">
         <v>20</v>
       </c>
@@ -1042,8 +1559,8 @@
       <c r="H30" t="s">
         <v>36</v>
       </c>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
       <c r="N30" t="s">
         <v>21</v>
       </c>
@@ -1084,11 +1601,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31A7BC2-D259-5943-B5A3-5653F97DB072}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -1099,8 +1616,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17" customHeight="1">
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>

</xml_diff>